<commit_message>
more couchdb code edits
</commit_message>
<xml_diff>
--- a/Docs/Excel/UI Proto.xlsx
+++ b/Docs/Excel/UI Proto.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16215" windowHeight="16155" tabRatio="676" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16215" windowHeight="16155" tabRatio="676" firstSheet="1" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Text Outline" sheetId="3" r:id="rId1"/>
@@ -23,6 +23,8 @@
     <sheet name="WorkOrderReportTS" sheetId="18" r:id="rId9"/>
     <sheet name="Word Lists" sheetId="19" r:id="rId10"/>
     <sheet name="UserConfig" sheetId="20" r:id="rId11"/>
+    <sheet name="UserConfig cont." sheetId="21" r:id="rId12"/>
+    <sheet name="TestData" sheetId="22" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15514" uniqueCount="2988">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15942" uniqueCount="3098">
   <si>
     <t>Login</t>
   </si>
@@ -8998,6 +9000,336 @@
   </si>
   <si>
     <t>firstName</t>
+  </si>
+  <si>
+    <t>Indx</t>
+  </si>
+  <si>
+    <t>userClassIndx</t>
+  </si>
+  <si>
+    <t>locPrimryIndx</t>
+  </si>
+  <si>
+    <t>locScndryIndx</t>
+  </si>
+  <si>
+    <t>clntCmpnyIndx</t>
+  </si>
+  <si>
+    <t>pyrlClassIndx</t>
+  </si>
+  <si>
+    <t>idUClassIndx</t>
+  </si>
+  <si>
+    <t>idLocPrmIndx</t>
+  </si>
+  <si>
+    <t>idLoc2ndIndx</t>
+  </si>
+  <si>
+    <t>idCompanyIndx</t>
+  </si>
+  <si>
+    <t>firstName?</t>
+  </si>
+  <si>
+    <t>lastName?</t>
+  </si>
+  <si>
+    <t>email?</t>
+  </si>
+  <si>
+    <t>userClass?</t>
+  </si>
+  <si>
+    <t>locPrimry?</t>
+  </si>
+  <si>
+    <t>locScndry?</t>
+  </si>
+  <si>
+    <t>clntCmpny?</t>
+  </si>
+  <si>
+    <t>pyrlClass?</t>
+  </si>
+  <si>
+    <t>idUClass?</t>
+  </si>
+  <si>
+    <t>idLocPrm?</t>
+  </si>
+  <si>
+    <t>idLoc2nd?</t>
+  </si>
+  <si>
+    <t>idCompany?</t>
+  </si>
+  <si>
+    <t>userClassIndx?</t>
+  </si>
+  <si>
+    <t>locPrimryIndx?</t>
+  </si>
+  <si>
+    <t>locScndryIndx?</t>
+  </si>
+  <si>
+    <t>clntCmpnyIndx?</t>
+  </si>
+  <si>
+    <t>pyrlClassIndx?</t>
+  </si>
+  <si>
+    <t>idUClassIndx?</t>
+  </si>
+  <si>
+    <t>idLocPrmIndx?</t>
+  </si>
+  <si>
+    <t>idLoc2ndIndx?</t>
+  </si>
+  <si>
+    <t>idCompanyIndx?</t>
+  </si>
+  <si>
+    <t>public</t>
+  </si>
+  <si>
+    <t>setuserClass</t>
+  </si>
+  <si>
+    <t>setlocPrimry</t>
+  </si>
+  <si>
+    <t>setlocScndry</t>
+  </si>
+  <si>
+    <t>setclntCmpny</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t>this.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ) { </t>
+  </si>
+  <si>
+    <t xml:space="preserve">( </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ]; }</t>
+  </si>
+  <si>
+    <t>setIdUClass</t>
+  </si>
+  <si>
+    <t>setIdLocPrm</t>
+  </si>
+  <si>
+    <t>setIdLoc2nd</t>
+  </si>
+  <si>
+    <t>setIdCompany</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>toString();</t>
+  </si>
+  <si>
+    <t>dbIdPrefix</t>
+  </si>
+  <si>
+    <t>usrIdStr</t>
+  </si>
+  <si>
+    <t>this.usr this.a + this.b + this.c + this.d;</t>
+  </si>
+  <si>
+    <t>this.lastName + '_' + this.firstName;</t>
+  </si>
+  <si>
+    <t>Stephen</t>
+  </si>
+  <si>
+    <t>Gonzalez</t>
+  </si>
+  <si>
+    <t>let idUClass = 63;</t>
+  </si>
+  <si>
+    <t>let idLocPrm = 92;</t>
+  </si>
+  <si>
+    <t>let idLoc2nd = 33;</t>
+  </si>
+  <si>
+    <t>let idCompany = 33;</t>
+  </si>
+  <si>
+    <t>let a = idUClass.toString();</t>
+  </si>
+  <si>
+    <t>let b = idLocPrm.toString();</t>
+  </si>
+  <si>
+    <t>let c = idLoc2nd.toString();</t>
+  </si>
+  <si>
+    <t>let d = idCompany.toString();</t>
+  </si>
+  <si>
+    <t>let dbIdPrefix = usrIdStr + a + b + c + d;</t>
+  </si>
+  <si>
+    <t>let usrIdStr   = lastName + '_' + firstName;</t>
+  </si>
+  <si>
+    <t>let firstName = 'Stephen';</t>
+  </si>
+  <si>
+    <t>let lastName = 'Gonzalez';</t>
+  </si>
+  <si>
+    <t>middleName</t>
+  </si>
+  <si>
+    <t>namePrefix</t>
+  </si>
+  <si>
+    <t>nameSuffix</t>
+  </si>
+  <si>
+    <t>: string;</t>
+  </si>
+  <si>
+    <t>export class UserComponent {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public firstName     : string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public lastName      : string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public email         : string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public userClass     : string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public locPrimry     : string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public locScndry     : string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public clntCmpny     : string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public pyrlClass     : string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public idUClass      : string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public idLocPrm      : string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public idLoc2nd      : string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public idCompany     : string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public userClassIndx : number;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public locPrimryIndx : number;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public locScndryIndx : number;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public clntCmpnyIndx : number;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public pyrlClassIndx : number;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public idUClassIndx  : string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public idLocPrmIndx  : string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public idLoc2ndIndx  : string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public idCompanyIndx : string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public usr           : string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public dbIdPrefix    : string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public a             : string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public b             : string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public c             : string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public d             : string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public usrIdStr      : string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public dateStr       : string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public middleName    : string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public namePrefix    : string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      public nameSuffix    : string;</t>
+  </si>
+  <si>
+    <t>let nameSuffix = '';</t>
+  </si>
+  <si>
+    <t>let namePrefix = '';</t>
+  </si>
+  <si>
+    <t>let middleName = 'A';</t>
+  </si>
+  <si>
+    <t>let docContents = Lorem ipsum Quis consequat nulla aliquip dolor pariatur consequat.</t>
   </si>
 </sst>
 </file>
@@ -14193,10 +14525,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U75"/>
+  <dimension ref="A1:AA75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -14217,7 +14549,7 @@
     <col min="18" max="16384" width="9" style="483"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15">
+    <row r="1" spans="1:27" ht="15">
       <c r="A1" s="4" t="s">
         <v>2981</v>
       </c>
@@ -14255,7 +14587,7 @@
         <v>2983</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15">
+    <row r="2" spans="1:27" ht="15">
       <c r="A2" s="4"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -14305,7 +14637,7 @@
         <v>2984</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="15">
+    <row r="3" spans="1:27" ht="15">
       <c r="A3" s="4"/>
       <c r="B3"/>
       <c r="C3"/>
@@ -14352,7 +14684,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15">
+    <row r="4" spans="1:27" ht="15">
       <c r="A4" s="4"/>
       <c r="B4"/>
       <c r="C4"/>
@@ -14399,7 +14731,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15">
+    <row r="5" spans="1:27" ht="15">
       <c r="A5" s="4"/>
       <c r="B5"/>
       <c r="C5"/>
@@ -14446,7 +14778,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15">
+    <row r="6" spans="1:27" ht="15">
       <c r="A6" s="4"/>
       <c r="B6"/>
       <c r="C6"/>
@@ -14493,7 +14825,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15">
+    <row r="7" spans="1:27" ht="15">
       <c r="A7" s="4"/>
       <c r="B7"/>
       <c r="C7"/>
@@ -14537,7 +14869,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15">
+    <row r="8" spans="1:27" ht="15">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
@@ -14568,7 +14900,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="15">
+    <row r="9" spans="1:27" ht="15">
       <c r="A9" s="4"/>
       <c r="B9"/>
       <c r="C9"/>
@@ -14597,7 +14929,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15">
+    <row r="10" spans="1:27" ht="15">
       <c r="A10" s="4" t="s">
         <v>2981</v>
       </c>
@@ -14609,7 +14941,7 @@
       </c>
       <c r="K10" s="481"/>
     </row>
-    <row r="11" spans="1:21" ht="15">
+    <row r="11" spans="1:27" ht="15">
       <c r="A11" s="4"/>
       <c r="B11"/>
       <c r="C11"/>
@@ -14632,7 +14964,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15">
+    <row r="12" spans="1:27" ht="15">
       <c r="A12" s="4"/>
       <c r="B12"/>
       <c r="C12"/>
@@ -14657,7 +14989,7 @@
       <c r="N12" s="2"/>
       <c r="Q12" s="485"/>
     </row>
-    <row r="13" spans="1:21" ht="15">
+    <row r="13" spans="1:27" ht="15">
       <c r="A13" s="4"/>
       <c r="B13"/>
       <c r="C13"/>
@@ -14679,20 +15011,35 @@
       <c r="I13" s="484" t="s">
         <v>21</v>
       </c>
-      <c r="Q13" s="483" t="s">
+      <c r="Q13" s="4" t="s">
+        <v>2998</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>2529</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="W13" s="483" t="s">
+        <v>3019</v>
+      </c>
+      <c r="X13" s="2" t="s">
         <v>2987</v>
       </c>
-      <c r="R13" s="483" t="s">
-        <v>2980</v>
-      </c>
-      <c r="S13" s="483" t="s">
+      <c r="Y13" s="483" t="s">
+        <v>560</v>
+      </c>
+      <c r="Z13" s="4" t="s">
         <v>2529</v>
       </c>
-      <c r="T13" s="483" t="s">
+      <c r="AA13" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15">
+    <row r="14" spans="1:27" ht="15">
       <c r="A14" s="4"/>
       <c r="B14"/>
       <c r="C14"/>
@@ -14714,20 +15061,35 @@
       <c r="I14" s="484" t="s">
         <v>21</v>
       </c>
-      <c r="Q14" s="483" t="s">
+      <c r="Q14" s="4" t="s">
+        <v>2999</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>2529</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="W14" s="483" t="s">
+        <v>3019</v>
+      </c>
+      <c r="X14" s="2" t="s">
         <v>2986</v>
       </c>
-      <c r="R14" s="483" t="s">
-        <v>2980</v>
-      </c>
-      <c r="S14" s="483" t="s">
+      <c r="Y14" s="483" t="s">
+        <v>560</v>
+      </c>
+      <c r="Z14" s="4" t="s">
         <v>2529</v>
       </c>
-      <c r="T14" s="483" t="s">
+      <c r="AA14" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15">
+    <row r="15" spans="1:27" ht="15">
       <c r="A15" s="4"/>
       <c r="B15"/>
       <c r="C15"/>
@@ -14746,56 +15108,119 @@
       <c r="H15" s="484">
         <v>24</v>
       </c>
-      <c r="Q15" s="483" t="s">
+      <c r="N15" s="481" t="s">
+        <v>2970</v>
+      </c>
+      <c r="O15" s="483" t="s">
+        <v>2988</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>3000</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>2529</v>
+      </c>
+      <c r="T15" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="W15" s="483" t="s">
+        <v>3019</v>
+      </c>
+      <c r="X15" s="2" t="s">
         <v>2985</v>
       </c>
-      <c r="R15" s="483" t="s">
-        <v>2980</v>
-      </c>
-      <c r="S15" s="483" t="s">
+      <c r="Y15" s="483" t="s">
+        <v>560</v>
+      </c>
+      <c r="Z15" s="4" t="s">
         <v>2529</v>
       </c>
-      <c r="T15" s="483" t="s">
+      <c r="AA15" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15">
+    <row r="16" spans="1:27" ht="15">
       <c r="A16" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
-      <c r="Q16" s="481" t="s">
+      <c r="N16" s="481" t="s">
+        <v>2971</v>
+      </c>
+      <c r="O16" s="483" t="s">
+        <v>2988</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>3001</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>2529</v>
+      </c>
+      <c r="T16" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="W16" s="483" t="s">
+        <v>3019</v>
+      </c>
+      <c r="X16" s="2" t="s">
         <v>2970</v>
       </c>
-      <c r="R16" s="483" t="s">
-        <v>2980</v>
-      </c>
-      <c r="S16" s="481" t="s">
-        <v>2968</v>
-      </c>
-      <c r="T16" s="483" t="s">
+      <c r="Y16" s="483" t="s">
+        <v>560</v>
+      </c>
+      <c r="Z16" s="4" t="s">
+        <v>2529</v>
+      </c>
+      <c r="AA16" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="15">
+    <row r="17" spans="1:27" ht="15">
       <c r="A17" s="4"/>
       <c r="B17"/>
       <c r="C17"/>
-      <c r="Q17" s="481" t="s">
+      <c r="N17" s="481" t="s">
+        <v>2972</v>
+      </c>
+      <c r="O17" s="483" t="s">
+        <v>2988</v>
+      </c>
+      <c r="Q17" s="4" t="s">
+        <v>3002</v>
+      </c>
+      <c r="R17" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="S17" s="4" t="s">
+        <v>2529</v>
+      </c>
+      <c r="T17" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="W17" s="483" t="s">
+        <v>3019</v>
+      </c>
+      <c r="X17" s="2" t="s">
         <v>2971</v>
       </c>
-      <c r="R17" s="483" t="s">
-        <v>2980</v>
-      </c>
-      <c r="S17" s="481" t="s">
-        <v>2964</v>
-      </c>
-      <c r="T17" s="483" t="s">
+      <c r="Y17" s="483" t="s">
+        <v>560</v>
+      </c>
+      <c r="Z17" s="4" t="s">
+        <v>2529</v>
+      </c>
+      <c r="AA17" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="15">
+    <row r="18" spans="1:27" ht="15">
       <c r="A18" s="4" t="s">
         <v>2981</v>
       </c>
@@ -14805,20 +15230,41 @@
       <c r="C18" s="4" t="s">
         <v>2982</v>
       </c>
-      <c r="Q18" s="481" t="s">
+      <c r="N18" s="481" t="s">
+        <v>2973</v>
+      </c>
+      <c r="O18" s="483" t="s">
+        <v>2988</v>
+      </c>
+      <c r="Q18" s="4" t="s">
+        <v>3003</v>
+      </c>
+      <c r="R18" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="S18" s="4" t="s">
+        <v>2529</v>
+      </c>
+      <c r="T18" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="W18" s="483" t="s">
+        <v>3019</v>
+      </c>
+      <c r="X18" s="2" t="s">
         <v>2972</v>
       </c>
-      <c r="R18" s="483" t="s">
-        <v>2980</v>
-      </c>
-      <c r="S18" s="481" t="s">
-        <v>2965</v>
-      </c>
-      <c r="T18" s="483" t="s">
+      <c r="Y18" s="483" t="s">
+        <v>560</v>
+      </c>
+      <c r="Z18" s="4" t="s">
+        <v>2529</v>
+      </c>
+      <c r="AA18" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="15">
+    <row r="19" spans="1:27" ht="15">
       <c r="A19" s="4"/>
       <c r="B19"/>
       <c r="C19"/>
@@ -14840,20 +15286,41 @@
       <c r="I19" s="484" t="s">
         <v>21</v>
       </c>
-      <c r="Q19" s="481" t="s">
+      <c r="N19" s="481" t="s">
+        <v>2974</v>
+      </c>
+      <c r="O19" s="483" t="s">
+        <v>2988</v>
+      </c>
+      <c r="Q19" s="4" t="s">
+        <v>3004</v>
+      </c>
+      <c r="R19" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="S19" s="4" t="s">
+        <v>2529</v>
+      </c>
+      <c r="T19" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="W19" s="483" t="s">
+        <v>3019</v>
+      </c>
+      <c r="X19" s="2" t="s">
         <v>2973</v>
       </c>
-      <c r="R19" s="483" t="s">
-        <v>2980</v>
-      </c>
-      <c r="S19" s="481" t="s">
-        <v>2966</v>
-      </c>
-      <c r="T19" s="483" t="s">
+      <c r="Y19" s="483" t="s">
+        <v>560</v>
+      </c>
+      <c r="Z19" s="4" t="s">
+        <v>2529</v>
+      </c>
+      <c r="AA19" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="15">
+    <row r="20" spans="1:27" ht="15">
       <c r="A20" s="4"/>
       <c r="B20"/>
       <c r="C20"/>
@@ -14875,20 +15342,41 @@
       <c r="I20" s="484" t="s">
         <v>21</v>
       </c>
-      <c r="Q20" s="481" t="s">
+      <c r="N20" s="481" t="s">
+        <v>2975</v>
+      </c>
+      <c r="O20" s="483" t="s">
+        <v>2988</v>
+      </c>
+      <c r="Q20" s="4" t="s">
+        <v>3005</v>
+      </c>
+      <c r="R20" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="S20" s="4" t="s">
+        <v>2529</v>
+      </c>
+      <c r="T20" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="W20" s="483" t="s">
+        <v>3019</v>
+      </c>
+      <c r="X20" s="2" t="s">
         <v>2974</v>
       </c>
-      <c r="R20" s="483" t="s">
-        <v>2980</v>
-      </c>
-      <c r="S20" s="481" t="s">
-        <v>2967</v>
-      </c>
-      <c r="T20" s="483" t="s">
+      <c r="Y20" s="483" t="s">
+        <v>560</v>
+      </c>
+      <c r="Z20" s="4" t="s">
+        <v>2529</v>
+      </c>
+      <c r="AA20" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="15">
+    <row r="21" spans="1:27" ht="15">
       <c r="A21" s="4"/>
       <c r="B21"/>
       <c r="C21"/>
@@ -14910,20 +15398,41 @@
       <c r="I21" s="484" t="s">
         <v>21</v>
       </c>
-      <c r="Q21" s="481" t="s">
+      <c r="N21" s="481" t="s">
+        <v>2976</v>
+      </c>
+      <c r="O21" s="483" t="s">
+        <v>2988</v>
+      </c>
+      <c r="Q21" s="4" t="s">
+        <v>3006</v>
+      </c>
+      <c r="R21" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="S21" s="4" t="s">
+        <v>2529</v>
+      </c>
+      <c r="T21" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="W21" s="483" t="s">
+        <v>3019</v>
+      </c>
+      <c r="X21" s="2" t="s">
         <v>2975</v>
       </c>
-      <c r="R21" s="483" t="s">
-        <v>2980</v>
-      </c>
-      <c r="S21" s="481" t="s">
-        <v>2969</v>
-      </c>
-      <c r="T21" s="483" t="s">
+      <c r="Y21" s="483" t="s">
+        <v>560</v>
+      </c>
+      <c r="Z21" s="4" t="s">
+        <v>2529</v>
+      </c>
+      <c r="AA21" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="15">
+    <row r="22" spans="1:27" ht="15">
       <c r="A22" s="4"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -14945,20 +15454,41 @@
       <c r="I22" s="484" t="s">
         <v>21</v>
       </c>
-      <c r="Q22" s="481" t="s">
+      <c r="N22" s="481" t="s">
+        <v>2977</v>
+      </c>
+      <c r="O22" s="483" t="s">
+        <v>2988</v>
+      </c>
+      <c r="Q22" s="4" t="s">
+        <v>3007</v>
+      </c>
+      <c r="R22" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="S22" s="4" t="s">
+        <v>2529</v>
+      </c>
+      <c r="T22" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="W22" s="483" t="s">
+        <v>3019</v>
+      </c>
+      <c r="X22" s="2" t="s">
         <v>2976</v>
       </c>
-      <c r="R22" s="483" t="s">
-        <v>2980</v>
-      </c>
-      <c r="S22" s="481" t="s">
-        <v>2963</v>
-      </c>
-      <c r="T22" s="483" t="s">
+      <c r="Y22" s="483" t="s">
+        <v>560</v>
+      </c>
+      <c r="Z22" s="4" t="s">
+        <v>2529</v>
+      </c>
+      <c r="AA22" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="15">
+    <row r="23" spans="1:27" ht="15">
       <c r="A23" s="4"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -14980,20 +15510,41 @@
       <c r="I23" s="484" t="s">
         <v>21</v>
       </c>
-      <c r="Q23" s="481" t="s">
+      <c r="N23" s="481" t="s">
+        <v>2978</v>
+      </c>
+      <c r="O23" s="483" t="s">
+        <v>2988</v>
+      </c>
+      <c r="Q23" s="4" t="s">
+        <v>3008</v>
+      </c>
+      <c r="R23" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="S23" s="4" t="s">
+        <v>2529</v>
+      </c>
+      <c r="T23" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="W23" s="483" t="s">
+        <v>3019</v>
+      </c>
+      <c r="X23" s="2" t="s">
         <v>2977</v>
       </c>
-      <c r="R23" s="483" t="s">
-        <v>2980</v>
-      </c>
-      <c r="S23" s="481" t="s">
-        <v>2961</v>
-      </c>
-      <c r="T23" s="483" t="s">
+      <c r="Y23" s="483" t="s">
+        <v>560</v>
+      </c>
+      <c r="Z23" s="4" t="s">
+        <v>2529</v>
+      </c>
+      <c r="AA23" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="15">
+    <row r="24" spans="1:27" ht="15">
       <c r="A24" s="4"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -15012,32 +15563,101 @@
       <c r="H24" s="484">
         <v>35</v>
       </c>
-      <c r="Q24" s="481" t="s">
+      <c r="Q24" s="4" t="s">
+        <v>3009</v>
+      </c>
+      <c r="R24" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="S24" s="4" t="s">
+        <v>2529</v>
+      </c>
+      <c r="T24" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="W24" s="483" t="s">
+        <v>3019</v>
+      </c>
+      <c r="X24" s="2" t="s">
         <v>2978</v>
       </c>
-      <c r="R24" s="483" t="s">
-        <v>2980</v>
-      </c>
-      <c r="S24" s="481" t="s">
-        <v>2962</v>
-      </c>
-      <c r="T24" s="483" t="s">
+      <c r="Y24" s="483" t="s">
+        <v>560</v>
+      </c>
+      <c r="Z24" s="4" t="s">
+        <v>2529</v>
+      </c>
+      <c r="AA24" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="15">
+    <row r="25" spans="1:27" ht="15">
       <c r="A25" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B25"/>
       <c r="C25"/>
-    </row>
-    <row r="26" spans="1:20" ht="15">
+      <c r="Q25" s="4" t="s">
+        <v>3010</v>
+      </c>
+      <c r="R25" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="S25" s="4" t="s">
+        <v>2533</v>
+      </c>
+      <c r="T25" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="W25" s="483" t="s">
+        <v>3019</v>
+      </c>
+      <c r="X25" s="2" t="s">
+        <v>2989</v>
+      </c>
+      <c r="Y25" s="483" t="s">
+        <v>560</v>
+      </c>
+      <c r="Z25" s="4" t="s">
+        <v>2533</v>
+      </c>
+      <c r="AA25" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" ht="15">
       <c r="A26" s="4"/>
       <c r="B26"/>
       <c r="C26"/>
-    </row>
-    <row r="27" spans="1:20" ht="15">
+      <c r="Q26" s="4" t="s">
+        <v>3011</v>
+      </c>
+      <c r="R26" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="S26" s="4" t="s">
+        <v>2533</v>
+      </c>
+      <c r="T26" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="W26" s="483" t="s">
+        <v>3019</v>
+      </c>
+      <c r="X26" s="2" t="s">
+        <v>2990</v>
+      </c>
+      <c r="Y26" s="483" t="s">
+        <v>560</v>
+      </c>
+      <c r="Z26" s="4" t="s">
+        <v>2533</v>
+      </c>
+      <c r="AA26" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" ht="15">
       <c r="A27" s="4" t="s">
         <v>2981</v>
       </c>
@@ -15047,8 +15667,35 @@
       <c r="C27" s="4" t="s">
         <v>2982</v>
       </c>
-    </row>
-    <row r="28" spans="1:20" ht="15">
+      <c r="Q27" s="4" t="s">
+        <v>3012</v>
+      </c>
+      <c r="R27" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="S27" s="4" t="s">
+        <v>2533</v>
+      </c>
+      <c r="T27" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="W27" s="483" t="s">
+        <v>3019</v>
+      </c>
+      <c r="X27" s="2" t="s">
+        <v>2991</v>
+      </c>
+      <c r="Y27" s="483" t="s">
+        <v>560</v>
+      </c>
+      <c r="Z27" s="4" t="s">
+        <v>2533</v>
+      </c>
+      <c r="AA27" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" ht="15">
       <c r="A28" s="4"/>
       <c r="B28"/>
       <c r="C28"/>
@@ -15070,8 +15717,35 @@
       <c r="I28" s="484" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" ht="15">
+      <c r="Q28" s="4" t="s">
+        <v>3013</v>
+      </c>
+      <c r="R28" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="S28" s="4" t="s">
+        <v>2533</v>
+      </c>
+      <c r="T28" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="W28" s="483" t="s">
+        <v>3019</v>
+      </c>
+      <c r="X28" s="2" t="s">
+        <v>2992</v>
+      </c>
+      <c r="Y28" s="483" t="s">
+        <v>560</v>
+      </c>
+      <c r="Z28" s="4" t="s">
+        <v>2533</v>
+      </c>
+      <c r="AA28" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" ht="15">
       <c r="A29" s="4"/>
       <c r="B29"/>
       <c r="C29"/>
@@ -15093,8 +15767,35 @@
       <c r="I29" s="484" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="30" spans="1:20" ht="15">
+      <c r="Q29" s="4" t="s">
+        <v>3014</v>
+      </c>
+      <c r="R29" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="S29" s="4" t="s">
+        <v>2533</v>
+      </c>
+      <c r="T29" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="W29" s="483" t="s">
+        <v>3019</v>
+      </c>
+      <c r="X29" s="2" t="s">
+        <v>2993</v>
+      </c>
+      <c r="Y29" s="483" t="s">
+        <v>560</v>
+      </c>
+      <c r="Z29" s="4" t="s">
+        <v>2533</v>
+      </c>
+      <c r="AA29" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" ht="15">
       <c r="A30" s="4"/>
       <c r="B30"/>
       <c r="C30"/>
@@ -15113,20 +15814,101 @@
       <c r="H30" s="484">
         <v>42</v>
       </c>
-    </row>
-    <row r="31" spans="1:20" ht="15">
+      <c r="Q30" s="4" t="s">
+        <v>3015</v>
+      </c>
+      <c r="R30" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="S30" s="4" t="s">
+        <v>2533</v>
+      </c>
+      <c r="T30" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="W30" s="483" t="s">
+        <v>3019</v>
+      </c>
+      <c r="X30" s="2" t="s">
+        <v>2994</v>
+      </c>
+      <c r="Y30" s="483" t="s">
+        <v>560</v>
+      </c>
+      <c r="Z30" s="4" t="s">
+        <v>2533</v>
+      </c>
+      <c r="AA30" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" ht="15">
       <c r="A31" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
-    </row>
-    <row r="32" spans="1:20" ht="15">
+      <c r="Q31" s="4" t="s">
+        <v>3016</v>
+      </c>
+      <c r="R31" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="S31" s="4" t="s">
+        <v>2533</v>
+      </c>
+      <c r="T31" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="W31" s="483" t="s">
+        <v>3019</v>
+      </c>
+      <c r="X31" s="2" t="s">
+        <v>2995</v>
+      </c>
+      <c r="Y31" s="483" t="s">
+        <v>560</v>
+      </c>
+      <c r="Z31" s="4" t="s">
+        <v>2533</v>
+      </c>
+      <c r="AA31" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" ht="15">
       <c r="A32" s="4"/>
       <c r="B32"/>
       <c r="C32"/>
-    </row>
-    <row r="33" spans="1:9" ht="15">
+      <c r="Q32" s="4" t="s">
+        <v>3017</v>
+      </c>
+      <c r="R32" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="S32" s="4" t="s">
+        <v>2533</v>
+      </c>
+      <c r="T32" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="W32" s="483" t="s">
+        <v>3019</v>
+      </c>
+      <c r="X32" s="2" t="s">
+        <v>2996</v>
+      </c>
+      <c r="Y32" s="483" t="s">
+        <v>560</v>
+      </c>
+      <c r="Z32" s="4" t="s">
+        <v>2533</v>
+      </c>
+      <c r="AA32" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" ht="15">
       <c r="A33" s="4" t="s">
         <v>2981</v>
       </c>
@@ -15136,8 +15918,35 @@
       <c r="C33" s="4" t="s">
         <v>2982</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="15">
+      <c r="Q33" s="4" t="s">
+        <v>3018</v>
+      </c>
+      <c r="R33" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="S33" s="4" t="s">
+        <v>2533</v>
+      </c>
+      <c r="T33" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="W33" s="483" t="s">
+        <v>3019</v>
+      </c>
+      <c r="X33" s="2" t="s">
+        <v>2997</v>
+      </c>
+      <c r="Y33" s="483" t="s">
+        <v>560</v>
+      </c>
+      <c r="Z33" s="4" t="s">
+        <v>2533</v>
+      </c>
+      <c r="AA33" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" ht="15">
       <c r="A34" s="4"/>
       <c r="B34"/>
       <c r="C34"/>
@@ -15160,7 +15969,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15">
+    <row r="35" spans="1:27" ht="15">
       <c r="A35" s="4"/>
       <c r="B35"/>
       <c r="C35"/>
@@ -15183,7 +15992,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15">
+    <row r="36" spans="1:27" ht="15">
       <c r="A36" s="4"/>
       <c r="B36"/>
       <c r="C36"/>
@@ -15206,7 +16015,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15">
+    <row r="37" spans="1:27" ht="15">
       <c r="A37" s="4"/>
       <c r="B37"/>
       <c r="C37"/>
@@ -15229,7 +16038,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15">
+    <row r="38" spans="1:27" ht="15">
       <c r="A38" s="4"/>
       <c r="B38"/>
       <c r="C38"/>
@@ -15252,7 +16061,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15">
+    <row r="39" spans="1:27" ht="15">
       <c r="A39" s="4"/>
       <c r="B39"/>
       <c r="C39"/>
@@ -15275,7 +16084,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="15">
+    <row r="40" spans="1:27" ht="15">
       <c r="A40" s="4"/>
       <c r="B40"/>
       <c r="C40"/>
@@ -15298,7 +16107,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="15">
+    <row r="41" spans="1:27" ht="15">
       <c r="A41" s="4"/>
       <c r="B41"/>
       <c r="C41"/>
@@ -15318,19 +16127,19 @@
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="15">
+    <row r="42" spans="1:27" ht="15">
       <c r="A42" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B42"/>
       <c r="C42"/>
     </row>
-    <row r="43" spans="1:9" ht="15">
+    <row r="43" spans="1:27" ht="15">
       <c r="A43" s="4"/>
       <c r="B43"/>
       <c r="C43"/>
     </row>
-    <row r="44" spans="1:9" ht="15">
+    <row r="44" spans="1:27" ht="15">
       <c r="A44" s="4" t="s">
         <v>2981</v>
       </c>
@@ -15341,7 +16150,7 @@
         <v>2982</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="15">
+    <row r="45" spans="1:27" ht="15">
       <c r="A45" s="4"/>
       <c r="B45"/>
       <c r="C45"/>
@@ -15364,7 +16173,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="15">
+    <row r="46" spans="1:27" ht="15">
       <c r="A46" s="4"/>
       <c r="B46"/>
       <c r="C46"/>
@@ -15387,7 +16196,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="15">
+    <row r="47" spans="1:27" ht="15">
       <c r="A47" s="4"/>
       <c r="B47"/>
       <c r="C47"/>
@@ -15410,7 +16219,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="15">
+    <row r="48" spans="1:27" ht="15">
       <c r="A48" s="4"/>
       <c r="B48"/>
       <c r="C48"/>
@@ -15867,6 +16676,1030 @@
       <c r="A75" s="2"/>
       <c r="B75"/>
       <c r="C75"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z55"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2:Z11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="9" style="3"/>
+    <col min="5" max="5" width="13" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="3"/>
+    <col min="12" max="12" width="9.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" style="3"/>
+    <col min="15" max="15" width="2.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26">
+      <c r="A1" s="4" t="s">
+        <v>2987</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
+      <c r="A2" s="4" t="s">
+        <v>2986</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>2987</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>2527</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>3043</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>3055</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
+      <c r="A3" s="4" t="s">
+        <v>2985</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>2986</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>2527</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>3044</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>3056</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
+      <c r="A4" s="4" t="s">
+        <v>2970</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>3020</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>3027</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>2970</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>2980</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>2529</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>3026</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>3025</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>2970</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>2527</v>
+      </c>
+      <c r="N4" s="481" t="s">
+        <v>2968</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>3028</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>3025</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>2989</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>3029</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>2975</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>2527</v>
+      </c>
+      <c r="V4" s="3">
+        <f ca="1">ROUND(RAND()*100,0)</f>
+        <v>58</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z4" s="4" t="s">
+        <v>3045</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
+      <c r="A5" s="4" t="s">
+        <v>2971</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>3021</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>3027</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>2971</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>2980</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>2529</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>3026</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>3025</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>2971</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>2527</v>
+      </c>
+      <c r="N5" s="481" t="s">
+        <v>2964</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>3028</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>3025</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>2990</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>3029</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>2976</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>2527</v>
+      </c>
+      <c r="V5" s="3">
+        <f t="shared" ref="V5:V7" ca="1" si="0">ROUND(RAND()*100,0)</f>
+        <v>20</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>3046</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
+      <c r="A6" s="4" t="s">
+        <v>2972</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>3022</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>3027</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>2972</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>2980</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>2529</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>3026</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>3025</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>2972</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>2527</v>
+      </c>
+      <c r="N6" s="481" t="s">
+        <v>2965</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>3028</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>3025</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>2991</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>3029</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>2977</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>2527</v>
+      </c>
+      <c r="V6" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z6" s="4" t="s">
+        <v>3047</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
+      <c r="A7" s="4" t="s">
+        <v>2973</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>3023</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>3027</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>2973</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>2980</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>2529</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>3026</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>3025</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>2973</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>2527</v>
+      </c>
+      <c r="N7" s="481" t="s">
+        <v>2966</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>3028</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>3025</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>2992</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>3029</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>2978</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>2527</v>
+      </c>
+      <c r="V7" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z7" s="4" t="s">
+        <v>3048</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26">
+      <c r="A8" s="4" t="s">
+        <v>2974</v>
+      </c>
+      <c r="T8" s="4" t="s">
+        <v>3034</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>2527</v>
+      </c>
+      <c r="V8" s="4" t="s">
+        <v>2975</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>2507</v>
+      </c>
+      <c r="X8" s="4" t="s">
+        <v>3038</v>
+      </c>
+      <c r="Z8" s="4" t="s">
+        <v>3049</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
+      <c r="A9" s="4" t="s">
+        <v>2975</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>3030</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>3024</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>2975</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>2980</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>2533</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>3026</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>3025</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>2975</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>2527</v>
+      </c>
+      <c r="N9" s="481" t="s">
+        <v>2968</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>3028</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>3025</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>2994</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>3029</v>
+      </c>
+      <c r="T9" s="4" t="s">
+        <v>3035</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>2527</v>
+      </c>
+      <c r="V9" s="4" t="s">
+        <v>2976</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>2507</v>
+      </c>
+      <c r="X9" s="4" t="s">
+        <v>3038</v>
+      </c>
+      <c r="Z9" s="4" t="s">
+        <v>3050</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
+      <c r="A10" s="4" t="s">
+        <v>2976</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>3031</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>3024</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>2976</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>2980</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>2533</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>3026</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>3025</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>2976</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>2527</v>
+      </c>
+      <c r="N10" s="481" t="s">
+        <v>2964</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>3028</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>3025</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>2995</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>3029</v>
+      </c>
+      <c r="T10" s="4" t="s">
+        <v>3036</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>2527</v>
+      </c>
+      <c r="V10" s="4" t="s">
+        <v>2977</v>
+      </c>
+      <c r="W10" s="3" t="s">
+        <v>2507</v>
+      </c>
+      <c r="X10" s="4" t="s">
+        <v>3038</v>
+      </c>
+      <c r="Z10" s="4" t="s">
+        <v>3051</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
+      <c r="A11" s="4" t="s">
+        <v>2977</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>3032</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>3024</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>2977</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>2980</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>2533</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>3026</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>3025</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>2977</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>2527</v>
+      </c>
+      <c r="N11" s="481" t="s">
+        <v>2965</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>3028</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>3025</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>2996</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>3029</v>
+      </c>
+      <c r="T11" s="4" t="s">
+        <v>3037</v>
+      </c>
+      <c r="U11" s="3" t="s">
+        <v>2527</v>
+      </c>
+      <c r="V11" s="4" t="s">
+        <v>2978</v>
+      </c>
+      <c r="W11" s="3" t="s">
+        <v>2507</v>
+      </c>
+      <c r="X11" s="4" t="s">
+        <v>3038</v>
+      </c>
+      <c r="Z11" s="4" t="s">
+        <v>3052</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
+      <c r="A12" s="4" t="s">
+        <v>2978</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>3033</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>3024</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>2978</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>2980</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>2533</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>3026</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>3025</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>2978</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>2527</v>
+      </c>
+      <c r="N12" s="481" t="s">
+        <v>2966</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>3028</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>3025</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>2997</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>3029</v>
+      </c>
+      <c r="Z12" s="3" t="s">
+        <v>3054</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
+      <c r="A13" s="4" t="s">
+        <v>2989</v>
+      </c>
+      <c r="Z13" s="3" t="s">
+        <v>3053</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
+      <c r="A14" s="4" t="s">
+        <v>2990</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>3025</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>3034</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>2527</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>2975</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>2507</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>3038</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15" s="4" t="s">
+        <v>2991</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>3025</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>3035</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>2527</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>2976</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>2507</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>3038</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16" s="4" t="s">
+        <v>2992</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>3025</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>3036</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>2527</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>2977</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>2507</v>
+      </c>
+      <c r="P16" s="4" t="s">
+        <v>3038</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25">
+      <c r="A17" s="4" t="s">
+        <v>2993</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>3025</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>3037</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>2527</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>2978</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>2507</v>
+      </c>
+      <c r="P17" s="4" t="s">
+        <v>3038</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25">
+      <c r="A18" s="4" t="s">
+        <v>2994</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>3025</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>3040</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>2527</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>3042</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25">
+      <c r="A19" s="4" t="s">
+        <v>2995</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>3025</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>3039</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>2527</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>3041</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25">
+      <c r="A20" s="4" t="s">
+        <v>2996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25">
+      <c r="A21" s="4" t="s">
+        <v>2997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25">
+      <c r="A22" s="4" t="s">
+        <v>3057</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>3060</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:25">
+      <c r="A23" s="4" t="s">
+        <v>3058</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>3060</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="3" t="s">
+        <v>3061</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25">
+      <c r="A24" s="4" t="s">
+        <v>3059</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>3060</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="3" t="s">
+        <v>3062</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25">
+      <c r="E25" s="3" t="s">
+        <v>3063</v>
+      </c>
+      <c r="U25" s="4" t="s">
+        <v>3057</v>
+      </c>
+      <c r="V25" s="4" t="s">
+        <v>3058</v>
+      </c>
+      <c r="W25" s="4" t="s">
+        <v>3059</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25">
+      <c r="E26" s="4" t="s">
+        <v>3091</v>
+      </c>
+      <c r="U26" s="4"/>
+      <c r="V26" s="4"/>
+      <c r="W26" s="4"/>
+    </row>
+    <row r="27" spans="1:25">
+      <c r="E27" s="4" t="s">
+        <v>3092</v>
+      </c>
+      <c r="U27" s="4"/>
+      <c r="V27" s="4"/>
+      <c r="W27" s="4"/>
+    </row>
+    <row r="28" spans="1:25">
+      <c r="E28" s="4" t="s">
+        <v>3093</v>
+      </c>
+      <c r="U28" s="4"/>
+      <c r="V28" s="4"/>
+      <c r="W28" s="4"/>
+    </row>
+    <row r="29" spans="1:25">
+      <c r="E29" s="3" t="s">
+        <v>3064</v>
+      </c>
+      <c r="U29" s="2"/>
+    </row>
+    <row r="30" spans="1:25">
+      <c r="E30" s="3" t="s">
+        <v>3065</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25">
+      <c r="E31" s="3" t="s">
+        <v>3066</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25">
+      <c r="E32" s="3" t="s">
+        <v>3067</v>
+      </c>
+      <c r="X32" s="2"/>
+      <c r="Y32" s="2"/>
+    </row>
+    <row r="33" spans="5:5">
+      <c r="E33" s="3" t="s">
+        <v>3068</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5">
+      <c r="E34" s="3" t="s">
+        <v>3069</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5">
+      <c r="E35" s="3" t="s">
+        <v>3070</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5">
+      <c r="E36" s="3" t="s">
+        <v>3071</v>
+      </c>
+    </row>
+    <row r="37" spans="5:5">
+      <c r="E37" s="3" t="s">
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="38" spans="5:5">
+      <c r="E38" s="3" t="s">
+        <v>3073</v>
+      </c>
+    </row>
+    <row r="39" spans="5:5">
+      <c r="E39" s="3" t="s">
+        <v>3074</v>
+      </c>
+    </row>
+    <row r="40" spans="5:5">
+      <c r="E40" s="3" t="s">
+        <v>3075</v>
+      </c>
+    </row>
+    <row r="41" spans="5:5">
+      <c r="E41" s="3" t="s">
+        <v>3076</v>
+      </c>
+    </row>
+    <row r="42" spans="5:5">
+      <c r="E42" s="3" t="s">
+        <v>3077</v>
+      </c>
+    </row>
+    <row r="43" spans="5:5">
+      <c r="E43" s="3" t="s">
+        <v>3078</v>
+      </c>
+    </row>
+    <row r="44" spans="5:5">
+      <c r="E44" s="3" t="s">
+        <v>3079</v>
+      </c>
+    </row>
+    <row r="45" spans="5:5">
+      <c r="E45" s="3" t="s">
+        <v>3080</v>
+      </c>
+    </row>
+    <row r="46" spans="5:5">
+      <c r="E46" s="3" t="s">
+        <v>3081</v>
+      </c>
+    </row>
+    <row r="47" spans="5:5">
+      <c r="E47" s="3" t="s">
+        <v>3082</v>
+      </c>
+    </row>
+    <row r="48" spans="5:5">
+      <c r="E48" s="3" t="s">
+        <v>3083</v>
+      </c>
+    </row>
+    <row r="49" spans="5:5">
+      <c r="E49" s="3" t="s">
+        <v>3084</v>
+      </c>
+    </row>
+    <row r="50" spans="5:5">
+      <c r="E50" s="3" t="s">
+        <v>3085</v>
+      </c>
+    </row>
+    <row r="51" spans="5:5">
+      <c r="E51" s="3" t="s">
+        <v>3086</v>
+      </c>
+    </row>
+    <row r="52" spans="5:5">
+      <c r="E52" s="3" t="s">
+        <v>3087</v>
+      </c>
+    </row>
+    <row r="53" spans="5:5">
+      <c r="E53" s="3" t="s">
+        <v>3088</v>
+      </c>
+    </row>
+    <row r="54" spans="5:5">
+      <c r="E54" s="3" t="s">
+        <v>3089</v>
+      </c>
+    </row>
+    <row r="55" spans="5:5">
+      <c r="E55" s="3" t="s">
+        <v>3090</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="4" t="s">
+        <v>3055</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="4" t="s">
+        <v>3056</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="4" t="s">
+        <v>3095</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="4" t="s">
+        <v>3096</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="4" t="s">
+        <v>3094</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="4" t="s">
+        <v>3045</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="4" t="s">
+        <v>3046</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="4" t="s">
+        <v>3047</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="4" t="s">
+        <v>3048</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="4" t="s">
+        <v>3097</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added copy of org OnSite to Docs
reference for completing OnSiteX
</commit_message>
<xml_diff>
--- a/Docs/Excel/UI Proto.xlsx
+++ b/Docs/Excel/UI Proto.xlsx
@@ -61641,7 +61641,7 @@
       </c>
       <c r="V4" s="3">
         <f ca="1">ROUND(RAND()*100,0)</f>
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="W4" s="3" t="s">
         <v>71</v>
@@ -61704,7 +61704,7 @@
       </c>
       <c r="V5" s="3">
         <f t="shared" ref="V5:V7" ca="1" si="0">ROUND(RAND()*100,0)</f>
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="W5" s="3" t="s">
         <v>71</v>
@@ -61767,7 +61767,7 @@
       </c>
       <c r="V6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="W6" s="3" t="s">
         <v>71</v>
@@ -61830,7 +61830,7 @@
       </c>
       <c r="V7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="W7" s="3" t="s">
         <v>71</v>

</xml_diff>